<commit_message>
Update MeteoWind_IoT_Pro_Gen2 payload decoder.xlsx
</commit_message>
<xml_diff>
--- a/MeteoWind_IoT_Pro Gen2/MeteoWind_IoT_Pro_Gen2 payload decoder.xlsx
+++ b/MeteoWind_IoT_Pro Gen2/MeteoWind_IoT_Pro_Gen2 payload decoder.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavol\Documents\GitHub\P_SRC_device_decoders\MeteoWind_IoT_Pro Gen2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavol\Documents\GitHub\FW_MeteoWind_IoT_Pro_Gen2\zDOC\payloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103B7EC5-67A2-4057-9B18-FFDF868868AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE085C0-865B-4960-AF6E-0ED0C57250BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -824,9 +824,6 @@
     <t>MeteoWind IoT ALARM message format 6 byte</t>
   </si>
   <si>
-    <t>18FA10E9B39180</t>
-  </si>
-  <si>
     <t>Debug_Flags</t>
   </si>
   <si>
@@ -1024,9 +1021,6 @@
     <t>MeteoWind IoT message format 10 byte</t>
   </si>
   <si>
-    <t>0582a1087050904b3114</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -1149,18 +1143,6 @@
     <t>Debug</t>
   </si>
   <si>
-    <t xml:space="preserve">    Hardware type - 0=test, 1=MeteoHelix, 2=MeteoWind, 3=MeteoRain, 4=MeteoAG, …</t>
-  </si>
-  <si>
-    <t>Major Firmware revision = 0…8     Example Firmware versioning like "0.03.009"</t>
-  </si>
-  <si>
-    <t>Minor Firmware revision = 0…255</t>
-  </si>
-  <si>
-    <t>Patch Firmware revision = 0…256</t>
-  </si>
-  <si>
     <t>{"IsHide":false,"HiddenInExcel":false,"SheetId":-1,"Name":"LoRa MeteoWind 10byte","Guid":"BW3A1M","Index":1,"VisibleRange":"","SheetTheme":{"TabColor":"","BodyColor":"","BodyImage":""},"IsPrintSheet":false}</t>
   </si>
   <si>
@@ -1203,9 +1185,6 @@
     <t>Upper lower</t>
   </si>
   <si>
-    <t>4442022700BE970004000000</t>
-  </si>
-  <si>
     <t>Anemo before Year 2023</t>
   </si>
   <si>
@@ -1216,6 +1195,27 @@
   </si>
   <si>
     <t>084D034D9800</t>
+  </si>
+  <si>
+    <t>049780C0D0D5975EC8028080</t>
+  </si>
+  <si>
+    <t>80B00BC00000000000000000</t>
+  </si>
+  <si>
+    <t>4442062700BE140004000000</t>
+  </si>
+  <si>
+    <t>Hardware type - 0=test, 1=MeteoHelix, 2=MeteoWind, 3=MeteoRain, 4=MeteoAG, …</t>
+  </si>
+  <si>
+    <t>Patch Firmware revision = 0…255</t>
+  </si>
+  <si>
+    <t>Minor Firmware revision = 0…63</t>
+  </si>
+  <si>
+    <t>Major Firmware revision = 0…7     Example Firmware versioning like "1.03.009"</t>
   </si>
 </sst>
 </file>
@@ -1748,29 +1748,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1785,12 +1766,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2091,50 +2091,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25 1025:1025" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
+      <c r="A1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
     </row>
     <row r="2" spans="1:25 1025:1025" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
@@ -2149,20 +2149,20 @@
       <c r="Y2" s="7"/>
     </row>
     <row r="3" spans="1:25 1025:1025" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
@@ -2181,41 +2181,41 @@
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
+      <c r="B4" s="78" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
     </row>
     <row r="5" spans="1:25 1025:1025" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="72" t="str">
+      <c r="B5" s="79" t="str">
         <f>CONCATENATE(B42,C42,D42,E42,F42,G42,H42,I42,J42,K42,L42,M42,N42,O42,P42,Q42,R42,S42,T42,U42,V42,W42,X42,Y42,Z42,AA42,AB42,AC42,AD42,AE42,AF42,AG42,AH42,AI42,AJ42,AK42)</f>
         <v>100111110000001111101000000010000000110000101110000010100000000010110100000000000101101000101101000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
     </row>
     <row r="6" spans="1:25 1025:1025" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -3139,7 +3139,7 @@
     </row>
     <row r="21" spans="1:26 1025:1025" x14ac:dyDescent="0.25">
       <c r="A21" s="67" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B21" s="50"/>
       <c r="C21" s="50"/>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="22" spans="1:26 1025:1025" x14ac:dyDescent="0.25">
       <c r="A22" s="67" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B22" s="50"/>
       <c r="C22" s="50"/>
@@ -3204,20 +3204,20 @@
       <c r="AMK22" s="1"/>
     </row>
     <row r="23" spans="1:26 1025:1025" x14ac:dyDescent="0.25">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="73"/>
-      <c r="L23" s="73"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="74"/>
+      <c r="K23" s="74"/>
+      <c r="L23" s="74"/>
       <c r="M23" s="51"/>
       <c r="N23" s="51"/>
       <c r="O23" s="51"/>
@@ -3264,52 +3264,52 @@
       <c r="Y24" s="51"/>
     </row>
     <row r="25" spans="1:26 1025:1025" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="74" t="s">
+      <c r="A25" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="74"/>
-      <c r="K25" s="74"/>
-      <c r="L25" s="74"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="75"/>
+      <c r="L25" s="75"/>
     </row>
     <row r="26" spans="1:26 1025:1025" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="74"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="74"/>
-      <c r="I26" s="74"/>
-      <c r="J26" s="74"/>
-      <c r="K26" s="74"/>
-      <c r="L26" s="74"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
+      <c r="J26" s="75"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="75"/>
     </row>
     <row r="27" spans="1:26 1025:1025" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="74" t="s">
+      <c r="A27" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="74"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="74"/>
-      <c r="K27" s="74"/>
-      <c r="L27" s="74"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="75"/>
     </row>
     <row r="28" spans="1:26 1025:1025" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -3424,50 +3424,50 @@
       <c r="L34" s="3"/>
     </row>
     <row r="35" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="70" t="s">
+      <c r="A35" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="70"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="70"/>
-      <c r="K35" s="70"/>
-      <c r="L35" s="70"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="69"/>
     </row>
     <row r="36" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="75" t="s">
+      <c r="A36" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="75"/>
-      <c r="C36" s="75"/>
-      <c r="D36" s="75"/>
-      <c r="E36" s="75"/>
-      <c r="F36" s="75"/>
-      <c r="G36" s="75"/>
-      <c r="H36" s="75"/>
-      <c r="I36" s="75"/>
-      <c r="J36" s="75"/>
-      <c r="K36" s="75"/>
-      <c r="L36" s="75"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="68"/>
+      <c r="J36" s="68"/>
+      <c r="K36" s="68"/>
+      <c r="L36" s="68"/>
     </row>
     <row r="37" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="70"/>
-      <c r="B37" s="70"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="70"/>
-      <c r="L37" s="70"/>
+      <c r="A37" s="69"/>
+      <c r="B37" s="69"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="69"/>
+      <c r="K37" s="69"/>
+      <c r="L37" s="69"/>
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
@@ -3487,33 +3487,33 @@
       <c r="R38" s="6"/>
     </row>
     <row r="39" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A39" s="76" t="s">
+      <c r="A39" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="76"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="76"/>
-      <c r="I39" s="76"/>
-      <c r="J39" s="76"/>
-      <c r="K39" s="76"/>
-      <c r="L39" s="76"/>
-      <c r="M39" s="76"/>
-      <c r="N39" s="76"/>
-      <c r="O39" s="76"/>
-      <c r="P39" s="76"/>
-      <c r="Q39" s="76"/>
-      <c r="R39" s="76"/>
-      <c r="S39" s="76"/>
-      <c r="T39" s="76"/>
-      <c r="U39" s="76"/>
-      <c r="V39" s="76"/>
-      <c r="W39" s="76"/>
-      <c r="X39" s="76"/>
-      <c r="Y39" s="76"/>
+      <c r="B39" s="70"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="70"/>
+      <c r="K39" s="70"/>
+      <c r="L39" s="70"/>
+      <c r="M39" s="70"/>
+      <c r="N39" s="70"/>
+      <c r="O39" s="70"/>
+      <c r="P39" s="70"/>
+      <c r="Q39" s="70"/>
+      <c r="R39" s="70"/>
+      <c r="S39" s="70"/>
+      <c r="T39" s="70"/>
+      <c r="U39" s="70"/>
+      <c r="V39" s="70"/>
+      <c r="W39" s="70"/>
+      <c r="X39" s="70"/>
+      <c r="Y39" s="70"/>
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -3944,26 +3944,26 @@
       <c r="P43" s="53"/>
     </row>
     <row r="44" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A44" s="77" t="s">
+      <c r="A44" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="B44" s="77"/>
-      <c r="C44" s="78" t="s">
+      <c r="B44" s="71"/>
+      <c r="C44" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="D44" s="78"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="79" t="s">
+      <c r="D44" s="72"/>
+      <c r="E44" s="72"/>
+      <c r="F44" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="G44" s="79"/>
-      <c r="H44" s="78" t="s">
+      <c r="G44" s="73"/>
+      <c r="H44" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="I44" s="78"/>
-      <c r="J44" s="78"/>
-      <c r="K44" s="78"/>
-      <c r="L44" s="78"/>
+      <c r="I44" s="72"/>
+      <c r="J44" s="72"/>
+      <c r="K44" s="72"/>
+      <c r="L44" s="72"/>
       <c r="M44" s="53"/>
       <c r="N44" s="53"/>
       <c r="O44" s="53"/>
@@ -3980,6 +3980,16 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="B5:O5"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="A35:L35"/>
     <mergeCell ref="A36:L36"/>
     <mergeCell ref="A37:L37"/>
     <mergeCell ref="A39:Y39"/>
@@ -3987,16 +3997,6 @@
     <mergeCell ref="C44:E44"/>
     <mergeCell ref="F44:G44"/>
     <mergeCell ref="H44:L44"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A27:L27"/>
-    <mergeCell ref="A35:L35"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="B5:O5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C44" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -4015,7 +4015,7 @@
   <dimension ref="A1:AMJ40"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:L4"/>
+      <selection activeCell="B5" sqref="B5:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4038,50 +4038,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
+      <c r="A1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
     </row>
     <row r="2" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7">
         <f>2^8</f>
@@ -4099,20 +4099,20 @@
       <c r="Y2" s="7"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
+      <c r="A3" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
@@ -4131,41 +4131,41 @@
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="80" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
+      <c r="B4" s="81" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="72" t="str">
+      <c r="B5" s="79" t="str">
         <f>CONCATENATE(B38,C38,D38,E38,F38,G38,H38,I38,J38,K38,L38,M38,N38,O38,P38,Q38,R38,S38,T38,U38,V38,W38,X38,Y38,Z38,AA38,AB38,AC38,AD38,AE38,AF38,AG38,AH38,AI38,AJ38,AK38)</f>
-        <v>000001011000001010100001000010000111000001010000100100000100101100110001000101000000000000000000000000000000000000000000000000000000000000000000</v>
-      </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
+        <v>000001001001011110000000110000001101000011010101100101110101111011001000000000101000000010000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -4233,31 +4233,31 @@
         <v>7</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="E7" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="61" t="s">
+      <c r="F7" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="61" t="s">
+      <c r="G7" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="61" t="s">
+      <c r="H7" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="G7" s="61" t="s">
+      <c r="I7" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="61" t="s">
+      <c r="J7" s="61" t="s">
         <v>85</v>
-      </c>
-      <c r="I7" s="61" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" s="61" t="s">
-        <v>87</v>
       </c>
       <c r="K7" s="62" t="s">
         <v>22</v>
@@ -4278,35 +4278,35 @@
       </c>
       <c r="C8" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>00010110000010101000010000</v>
+        <v>00010010010111100000001100</v>
       </c>
       <c r="D8" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>1000011100000101000010010</v>
+        <v>0000110100001101010110010</v>
       </c>
       <c r="E8" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>00</v>
+        <v>11</v>
       </c>
       <c r="F8" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>001</v>
+        <v>101</v>
       </c>
       <c r="G8" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>00101100</v>
+        <v>01111011</v>
       </c>
       <c r="H8" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>11000100</v>
+        <v>00100000</v>
       </c>
       <c r="I8" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>01010000</v>
+        <v>00001010</v>
       </c>
       <c r="J8" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>00000000</v>
+        <v>00000010</v>
       </c>
       <c r="K8" s="18" t="str">
         <f t="shared" si="1"/>
@@ -4340,35 +4340,35 @@
       </c>
       <c r="C9" s="18">
         <f ca="1">SUMPRODUCT(--MID(C8,LEN(C8)+1-ROW(INDIRECT("1:"&amp;LEN(C8))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(C8)))-1)))</f>
-        <v>5777936</v>
+        <v>4814860</v>
       </c>
       <c r="D9" s="18">
         <f ca="1">SUMPRODUCT(--MID(D8,LEN(D8)+1-ROW(INDIRECT("1:"&amp;LEN(D8))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(D8)))-1)))</f>
-        <v>17697298</v>
+        <v>1710770</v>
       </c>
       <c r="E9" s="18">
         <f t="shared" ref="E9:M9" si="2">BIN2DEC(E8)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F9" s="18">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G9" s="18">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="H9" s="18">
         <f t="shared" si="2"/>
-        <v>196</v>
+        <v>32</v>
       </c>
       <c r="I9" s="18">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J9" s="18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K9" s="18">
         <f t="shared" si="2"/>
@@ -4402,35 +4402,35 @@
       </c>
       <c r="C10" s="20">
         <f t="shared" ref="C10:O10" ca="1" si="3">C9*C12+C15</f>
-        <v>57.779360000000004</v>
+        <v>48.148600000000002</v>
       </c>
       <c r="D10" s="20">
         <f t="shared" ca="1" si="3"/>
-        <v>176.97298000000001</v>
+        <v>17.107700000000001</v>
       </c>
       <c r="E10" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F10" s="20">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G10" s="20">
         <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
+        <v>12.3</v>
       </c>
       <c r="H10" s="20">
         <f t="shared" si="3"/>
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="I10" s="20">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>2.5</v>
       </c>
       <c r="J10" s="20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K10" s="20">
         <f t="shared" si="3"/>
@@ -4470,13 +4470,13 @@
         <v>31</v>
       </c>
       <c r="E11" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="24" t="s">
         <v>88</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>90</v>
       </c>
       <c r="H11" s="24" t="s">
         <v>31</v>
@@ -4950,35 +4950,35 @@
       </c>
       <c r="C20" s="50">
         <f t="shared" ca="1" si="7"/>
-        <v>57.779360000000004</v>
+        <v>48.148600000000002</v>
       </c>
       <c r="D20" s="50">
         <f t="shared" ca="1" si="7"/>
-        <v>176.97298000000001</v>
+        <v>17.107700000000001</v>
       </c>
       <c r="E20" s="50">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F20" s="50">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G20" s="50">
         <f t="shared" si="7"/>
-        <v>4.4000000000000004</v>
+        <v>12.3</v>
       </c>
       <c r="H20" s="50">
         <f t="shared" si="7"/>
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="I20" s="50">
         <f t="shared" si="7"/>
-        <v>20</v>
+        <v>2.5</v>
       </c>
       <c r="J20" s="50">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K20" s="50">
         <f t="shared" si="7"/>
@@ -5002,43 +5002,43 @@
       </c>
     </row>
     <row r="21" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="75" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="75"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="75"/>
+      <c r="L21" s="75"/>
+    </row>
+    <row r="22" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="75" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
+      <c r="J22" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="74"/>
-      <c r="K21" s="74"/>
-      <c r="L21" s="74"/>
-    </row>
-    <row r="22" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="74" t="s">
+      <c r="K22" s="65" t="s">
         <v>92</v>
-      </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="J22" s="64" t="s">
-        <v>93</v>
-      </c>
-      <c r="K22" s="65" t="s">
-        <v>94</v>
       </c>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -5054,7 +5054,7 @@
     </row>
     <row r="24" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -5070,7 +5070,7 @@
     </row>
     <row r="25" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -5086,7 +5086,7 @@
     </row>
     <row r="26" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5102,7 +5102,7 @@
     </row>
     <row r="27" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -5118,82 +5118,82 @@
     </row>
     <row r="28" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="74"/>
-      <c r="B29" s="74"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="74"/>
-      <c r="L29" s="74"/>
+      <c r="A29" s="75"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="75"/>
+      <c r="L29" s="75"/>
     </row>
     <row r="30" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="74"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="74"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="74"/>
+      <c r="A30" s="75"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="75"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="75"/>
     </row>
     <row r="31" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="74"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="74"/>
-      <c r="I31" s="74"/>
-      <c r="J31" s="74"/>
-      <c r="K31" s="74"/>
-      <c r="L31" s="74"/>
+      <c r="A31" s="75"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="75"/>
+      <c r="I31" s="75"/>
+      <c r="J31" s="75"/>
+      <c r="K31" s="75"/>
+      <c r="L31" s="75"/>
     </row>
     <row r="32" spans="1:16" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="75" t="s">
+      <c r="A32" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="75"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="75"/>
-      <c r="K32" s="75"/>
-      <c r="L32" s="75"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="68"/>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A33" s="81" t="s">
-        <v>101</v>
-      </c>
-      <c r="B33" s="81"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="81"/>
-      <c r="G33" s="81"/>
-      <c r="H33" s="81"/>
-      <c r="I33" s="81"/>
-      <c r="J33" s="81"/>
-      <c r="K33" s="81"/>
-      <c r="L33" s="81"/>
+      <c r="A33" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="80"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="80"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="80"/>
+      <c r="K33" s="80"/>
+      <c r="L33" s="80"/>
       <c r="M33" s="53"/>
       <c r="N33" s="53"/>
       <c r="O33" s="53"/>
@@ -5202,20 +5202,20 @@
       <c r="R33" s="6"/>
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A34" s="81" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="81"/>
-      <c r="I34" s="81"/>
-      <c r="J34" s="81"/>
-      <c r="K34" s="81"/>
-      <c r="L34" s="81"/>
+      <c r="A34" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="80"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="80"/>
+      <c r="I34" s="80"/>
+      <c r="J34" s="80"/>
+      <c r="K34" s="80"/>
+      <c r="L34" s="80"/>
       <c r="M34" s="53"/>
       <c r="N34" s="53"/>
       <c r="O34" s="53"/>
@@ -5224,33 +5224,33 @@
       <c r="R34" s="6"/>
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A35" s="76" t="s">
+      <c r="A35" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="76"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="76"/>
-      <c r="J35" s="76"/>
-      <c r="K35" s="76"/>
-      <c r="L35" s="76"/>
-      <c r="M35" s="76"/>
-      <c r="N35" s="76"/>
-      <c r="O35" s="76"/>
-      <c r="P35" s="76"/>
-      <c r="Q35" s="76"/>
-      <c r="R35" s="76"/>
-      <c r="S35" s="76"/>
-      <c r="T35" s="76"/>
-      <c r="U35" s="76"/>
-      <c r="V35" s="76"/>
-      <c r="W35" s="76"/>
-      <c r="X35" s="76"/>
-      <c r="Y35" s="76"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="70"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="70"/>
+      <c r="K35" s="70"/>
+      <c r="L35" s="70"/>
+      <c r="M35" s="70"/>
+      <c r="N35" s="70"/>
+      <c r="O35" s="70"/>
+      <c r="P35" s="70"/>
+      <c r="Q35" s="70"/>
+      <c r="R35" s="70"/>
+      <c r="S35" s="70"/>
+      <c r="T35" s="70"/>
+      <c r="U35" s="70"/>
+      <c r="V35" s="70"/>
+      <c r="W35" s="70"/>
+      <c r="X35" s="70"/>
+      <c r="Y35" s="70"/>
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -5375,95 +5375,95 @@
       </c>
       <c r="C37" s="55" t="str">
         <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="D37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="E37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="F37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="G37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>C</v>
+      </c>
+      <c r="I37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>D</v>
+      </c>
+      <c r="K37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>D</v>
+      </c>
+      <c r="M37" s="55" t="str">
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="D37" s="55" t="str">
+      <c r="N37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="O37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="P37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="Q37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>E</v>
+      </c>
+      <c r="R37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>C</v>
+      </c>
+      <c r="S37" s="55" t="str">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="E37" s="55" t="str">
+      <c r="T37" s="55" t="str">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="U37" s="55" t="str">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="F37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>a</v>
-      </c>
-      <c r="G37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="H37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I37" s="55" t="str">
+      <c r="V37" s="55" t="str">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="J37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>7</v>
-      </c>
-      <c r="K37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="M37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="N37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>9</v>
-      </c>
-      <c r="O37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="Q37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>b</v>
-      </c>
-      <c r="R37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>3</v>
-      </c>
-      <c r="S37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="T37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="U37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="V37" s="55" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
       <c r="W37" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="X37" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="Y37" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="Z37" s="55" t="str">
         <f t="shared" si="8"/>
@@ -5524,91 +5524,91 @@
       </c>
       <c r="C38" s="54" t="str">
         <f t="shared" si="9"/>
+        <v>0100</v>
+      </c>
+      <c r="D38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>1001</v>
+      </c>
+      <c r="E38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>0111</v>
+      </c>
+      <c r="F38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+      <c r="G38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>0000</v>
+      </c>
+      <c r="H38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>1100</v>
+      </c>
+      <c r="I38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>0000</v>
+      </c>
+      <c r="J38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>1101</v>
+      </c>
+      <c r="K38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>0000</v>
+      </c>
+      <c r="L38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>1101</v>
+      </c>
+      <c r="M38" s="54" t="str">
+        <f t="shared" si="9"/>
         <v>0101</v>
       </c>
-      <c r="D38" s="54" t="str">
+      <c r="N38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>1001</v>
+      </c>
+      <c r="O38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>0111</v>
+      </c>
+      <c r="P38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>0101</v>
+      </c>
+      <c r="Q38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>1110</v>
+      </c>
+      <c r="R38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>1100</v>
+      </c>
+      <c r="S38" s="54" t="str">
         <f t="shared" si="9"/>
         <v>1000</v>
       </c>
-      <c r="E38" s="54" t="str">
+      <c r="T38" s="54" t="str">
+        <f t="shared" si="9"/>
+        <v>0000</v>
+      </c>
+      <c r="U38" s="54" t="str">
         <f t="shared" si="9"/>
         <v>0010</v>
       </c>
-      <c r="F38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>1010</v>
-      </c>
-      <c r="G38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>0001</v>
-      </c>
-      <c r="H38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>0000</v>
-      </c>
-      <c r="I38" s="54" t="str">
+      <c r="V38" s="54" t="str">
         <f t="shared" si="9"/>
         <v>1000</v>
       </c>
-      <c r="J38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>0111</v>
-      </c>
-      <c r="K38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>0000</v>
-      </c>
-      <c r="L38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>0101</v>
-      </c>
-      <c r="M38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>0000</v>
-      </c>
-      <c r="N38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>1001</v>
-      </c>
-      <c r="O38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>0000</v>
-      </c>
-      <c r="P38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>0100</v>
-      </c>
-      <c r="Q38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>1011</v>
-      </c>
-      <c r="R38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>0011</v>
-      </c>
-      <c r="S38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>0001</v>
-      </c>
-      <c r="T38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>0001</v>
-      </c>
-      <c r="U38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>0100</v>
-      </c>
-      <c r="V38" s="54" t="str">
-        <f t="shared" si="9"/>
-        <v>0000</v>
-      </c>
       <c r="W38" s="54" t="str">
         <f t="shared" si="9"/>
         <v>0000</v>
       </c>
       <c r="X38" s="54" t="str">
         <f t="shared" si="9"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="Y38" s="54" t="str">
         <f t="shared" si="9"/>
@@ -5681,26 +5681,26 @@
       <c r="P39" s="53"/>
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A40" s="77" t="s">
+      <c r="A40" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="77"/>
-      <c r="C40" s="78" t="s">
+      <c r="B40" s="71"/>
+      <c r="C40" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="78"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="79" t="s">
+      <c r="D40" s="72"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="G40" s="79"/>
-      <c r="H40" s="78" t="s">
+      <c r="G40" s="73"/>
+      <c r="H40" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="I40" s="78"/>
-      <c r="J40" s="78"/>
-      <c r="K40" s="78"/>
-      <c r="L40" s="78"/>
+      <c r="I40" s="72"/>
+      <c r="J40" s="72"/>
+      <c r="K40" s="72"/>
+      <c r="L40" s="72"/>
       <c r="M40" s="53"/>
       <c r="N40" s="53"/>
       <c r="O40" s="53"/>
@@ -5717,6 +5717,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="B5:O5"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="A31:L31"/>
     <mergeCell ref="A32:L32"/>
     <mergeCell ref="A33:L33"/>
     <mergeCell ref="A34:L34"/>
@@ -5725,16 +5735,6 @@
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="H40:L40"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="A30:L30"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="B5:O5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K22" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -5779,50 +5779,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
+      <c r="A1" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
     </row>
     <row r="2" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7">
         <f>2^8</f>
@@ -5840,20 +5840,20 @@
       <c r="Y2" s="7"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
+      <c r="A3" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
@@ -5872,41 +5872,41 @@
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="81" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="72" t="str">
+      <c r="B5" s="79" t="str">
         <f>CONCATENATE(B38,C38,D38,E38,F38,G38,H38,I38,J38,K38,L38,M38,N38,O38,P38,Q38,R38,S38,T38,U38,V38,W38,X38,Y38,Z38,AA38,AB38,AC38,AD38,AE38,AF38,AG38,AH38,AI38,AJ38,AK38)</f>
-        <v>010001000100001000000010001001110000000010111110100101110000000000000100000000000000000000000000000000000000000000000000000000000000000000000000</v>
-      </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
+        <v>010001000100001000000110001001110000000010111110000101000000000000000100000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -5974,40 +5974,40 @@
         <v>7</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="61" t="s">
+      <c r="F7" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="E7" s="61" t="s">
+      <c r="G7" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="F7" s="61" t="s">
+      <c r="H7" s="61" t="s">
         <v>106</v>
       </c>
-      <c r="G7" s="61" t="s">
+      <c r="I7" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="H7" s="61" t="s">
+      <c r="J7" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="I7" s="61" t="s">
+      <c r="K7" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="J7" s="61" t="s">
-        <v>110</v>
-      </c>
-      <c r="K7" s="62" t="s">
-        <v>111</v>
-      </c>
       <c r="L7" s="62" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="M7" s="62" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="N7" s="62"/>
       <c r="O7" s="14"/>
@@ -6035,7 +6035,7 @@
       </c>
       <c r="F8" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>00000010</v>
+        <v>00000110</v>
       </c>
       <c r="G8" s="18" t="str">
         <f t="shared" si="1"/>
@@ -6051,7 +6051,7 @@
       </c>
       <c r="J8" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>10010111</v>
+        <v>00010100</v>
       </c>
       <c r="K8" s="18" t="str">
         <f t="shared" si="1"/>
@@ -6097,7 +6097,7 @@
       </c>
       <c r="F9" s="18">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G9" s="18">
         <f t="shared" si="2"/>
@@ -6113,7 +6113,7 @@
       </c>
       <c r="J9" s="18">
         <f t="shared" si="2"/>
-        <v>151</v>
+        <v>20</v>
       </c>
       <c r="K9" s="18">
         <f t="shared" si="2"/>
@@ -6159,7 +6159,7 @@
       </c>
       <c r="F10" s="20">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G10" s="20">
         <f t="shared" si="3"/>
@@ -6175,7 +6175,7 @@
       </c>
       <c r="J10" s="20">
         <f t="shared" si="3"/>
-        <v>151</v>
+        <v>20</v>
       </c>
       <c r="K10" s="20">
         <f t="shared" si="3"/>
@@ -6707,7 +6707,7 @@
       </c>
       <c r="F20" s="50">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G20" s="50" t="str">
         <f>IF(LEN(DEC2HEX(G10))=1,CONCATENATE("0",DEC2HEX(G10) ),DEC2HEX(G10) )</f>
@@ -6723,7 +6723,7 @@
       </c>
       <c r="J20" s="50" t="str">
         <f t="shared" si="8"/>
-        <v>97</v>
+        <v>14</v>
       </c>
       <c r="K20" s="50">
         <f t="shared" si="7"/>
@@ -6747,37 +6747,37 @@
       </c>
     </row>
     <row r="21" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="74"/>
-      <c r="B21" s="74"/>
-      <c r="C21" s="74"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="74"/>
-      <c r="K21" s="74"/>
-      <c r="L21" s="74"/>
+      <c r="A21" s="75"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="75"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="75"/>
+      <c r="L21" s="75"/>
     </row>
     <row r="22" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="74" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
+      <c r="A22" s="75" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
       <c r="J22" s="64"/>
       <c r="K22" s="65"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -6793,7 +6793,7 @@
     </row>
     <row r="24" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -6809,7 +6809,7 @@
     </row>
     <row r="25" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -6855,78 +6855,78 @@
       <c r="A28" s="3"/>
     </row>
     <row r="29" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="74"/>
-      <c r="B29" s="74"/>
-      <c r="C29" s="74"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="74"/>
-      <c r="L29" s="74"/>
+      <c r="A29" s="75"/>
+      <c r="B29" s="75"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="75"/>
+      <c r="L29" s="75"/>
     </row>
     <row r="30" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="74"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="74"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="74"/>
+      <c r="A30" s="75"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="75"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="75"/>
     </row>
     <row r="31" spans="1:16" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="74"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="74"/>
-      <c r="I31" s="74"/>
-      <c r="J31" s="74"/>
-      <c r="K31" s="74"/>
-      <c r="L31" s="74"/>
+      <c r="A31" s="75"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="75"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="75"/>
+      <c r="I31" s="75"/>
+      <c r="J31" s="75"/>
+      <c r="K31" s="75"/>
+      <c r="L31" s="75"/>
     </row>
     <row r="32" spans="1:16" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="75" t="s">
+      <c r="A32" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="75"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="75"/>
-      <c r="K32" s="75"/>
-      <c r="L32" s="75"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="68"/>
     </row>
     <row r="33" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A33" s="81" t="s">
-        <v>101</v>
-      </c>
-      <c r="B33" s="81"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="81"/>
-      <c r="G33" s="81"/>
-      <c r="H33" s="81"/>
-      <c r="I33" s="81"/>
-      <c r="J33" s="81"/>
-      <c r="K33" s="81"/>
-      <c r="L33" s="81"/>
+      <c r="A33" s="80" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="80"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="80"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="80"/>
+      <c r="K33" s="80"/>
+      <c r="L33" s="80"/>
       <c r="M33" s="53"/>
       <c r="N33" s="53"/>
       <c r="O33" s="53"/>
@@ -6935,20 +6935,20 @@
       <c r="R33" s="6"/>
     </row>
     <row r="34" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A34" s="81" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="81"/>
-      <c r="I34" s="81"/>
-      <c r="J34" s="81"/>
-      <c r="K34" s="81"/>
-      <c r="L34" s="81"/>
+      <c r="A34" s="80" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="80"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="80"/>
+      <c r="I34" s="80"/>
+      <c r="J34" s="80"/>
+      <c r="K34" s="80"/>
+      <c r="L34" s="80"/>
       <c r="M34" s="53"/>
       <c r="N34" s="53"/>
       <c r="O34" s="53"/>
@@ -6957,33 +6957,33 @@
       <c r="R34" s="6"/>
     </row>
     <row r="35" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A35" s="76" t="s">
+      <c r="A35" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="76"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="76"/>
-      <c r="J35" s="76"/>
-      <c r="K35" s="76"/>
-      <c r="L35" s="76"/>
-      <c r="M35" s="76"/>
-      <c r="N35" s="76"/>
-      <c r="O35" s="76"/>
-      <c r="P35" s="76"/>
-      <c r="Q35" s="76"/>
-      <c r="R35" s="76"/>
-      <c r="S35" s="76"/>
-      <c r="T35" s="76"/>
-      <c r="U35" s="76"/>
-      <c r="V35" s="76"/>
-      <c r="W35" s="76"/>
-      <c r="X35" s="76"/>
-      <c r="Y35" s="76"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="70"/>
+      <c r="D35" s="70"/>
+      <c r="E35" s="70"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="70"/>
+      <c r="K35" s="70"/>
+      <c r="L35" s="70"/>
+      <c r="M35" s="70"/>
+      <c r="N35" s="70"/>
+      <c r="O35" s="70"/>
+      <c r="P35" s="70"/>
+      <c r="Q35" s="70"/>
+      <c r="R35" s="70"/>
+      <c r="S35" s="70"/>
+      <c r="T35" s="70"/>
+      <c r="U35" s="70"/>
+      <c r="V35" s="70"/>
+      <c r="W35" s="70"/>
+      <c r="X35" s="70"/>
+      <c r="Y35" s="70"/>
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -7124,12 +7124,12 @@
       </c>
       <c r="G37" s="55" t="str">
         <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="H37" s="55" t="str">
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="H37" s="55" t="str">
-        <f t="shared" si="9"/>
-        <v>2</v>
-      </c>
       <c r="I37" s="55" t="str">
         <f t="shared" si="9"/>
         <v>7</v>
@@ -7152,11 +7152,11 @@
       </c>
       <c r="N37" s="55" t="str">
         <f t="shared" si="9"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="O37" s="55" t="str">
         <f t="shared" si="9"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P37" s="55" t="str">
         <f t="shared" si="9"/>
@@ -7273,7 +7273,7 @@
       </c>
       <c r="G38" s="54" t="str">
         <f t="shared" si="10"/>
-        <v>0010</v>
+        <v>0110</v>
       </c>
       <c r="H38" s="54" t="str">
         <f t="shared" si="10"/>
@@ -7301,11 +7301,11 @@
       </c>
       <c r="N38" s="54" t="str">
         <f t="shared" si="10"/>
-        <v>1001</v>
+        <v>0001</v>
       </c>
       <c r="O38" s="54" t="str">
         <f t="shared" si="10"/>
-        <v>0111</v>
+        <v>0100</v>
       </c>
       <c r="P38" s="54" t="str">
         <f t="shared" si="10"/>
@@ -7414,26 +7414,26 @@
       <c r="P39" s="53"/>
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A40" s="77" t="s">
+      <c r="A40" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="B40" s="77"/>
-      <c r="C40" s="78" t="s">
+      <c r="B40" s="71"/>
+      <c r="C40" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="78"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="79" t="s">
+      <c r="D40" s="72"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="G40" s="79"/>
-      <c r="H40" s="78" t="s">
+      <c r="G40" s="73"/>
+      <c r="H40" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="I40" s="78"/>
-      <c r="J40" s="78"/>
-      <c r="K40" s="78"/>
-      <c r="L40" s="78"/>
+      <c r="I40" s="72"/>
+      <c r="J40" s="72"/>
+      <c r="K40" s="72"/>
+      <c r="L40" s="72"/>
       <c r="M40" s="53"/>
       <c r="N40" s="53"/>
       <c r="O40" s="53"/>
@@ -7450,6 +7450,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="B5:O5"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="A31:L31"/>
     <mergeCell ref="A32:L32"/>
     <mergeCell ref="A33:L33"/>
     <mergeCell ref="A34:L34"/>
@@ -7458,16 +7468,6 @@
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="H40:L40"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="A30:L30"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="B5:O5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A33" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
@@ -7505,50 +7505,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
-        <v>125</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
+      <c r="A1" s="76" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
     </row>
     <row r="2" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
@@ -7563,20 +7563,20 @@
       <c r="Y2" s="7"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="56"/>
@@ -7595,8 +7595,8 @@
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>69</v>
+      <c r="B4" s="19" t="s">
+        <v>129</v>
       </c>
       <c r="C4" s="57"/>
       <c r="D4" s="57"/>
@@ -7614,23 +7614,23 @@
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="72" t="str">
+      <c r="B5" s="79" t="str">
         <f>CONCATENATE(B34,C34,D34,E34,F34,G34,H34,I34,J34,K34,L34,M34,N34,O34,P34,Q34,R34,S34,T34,U34,V34,W34,X34,Y34,Z34,AA34,AB34,AC34,AD34,AE34,AF34,AG34,AH34,AI34,AJ34,AK34)</f>
-        <v>000110001111101000010000111010011011001110010001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
-      </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
+        <v>100000001011000000001011110000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
+      </c>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -7698,22 +7698,22 @@
         <v>7</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G7" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H7" s="17"/>
       <c r="J7" s="17"/>
@@ -7730,11 +7730,11 @@
       </c>
       <c r="B8" s="18" t="str">
         <f t="shared" ref="B8:O8" si="1">MID($B5,B6,B13)</f>
-        <v>00</v>
+        <v>10</v>
       </c>
       <c r="C8" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>011000111</v>
+        <v>000000101</v>
       </c>
       <c r="D8" s="18" t="str">
         <f t="shared" si="1"/>
@@ -7742,15 +7742,15 @@
       </c>
       <c r="E8" s="18" t="str">
         <f>MID($B5,E6,E13)</f>
-        <v>1010000</v>
+        <v>0000000</v>
       </c>
       <c r="F8" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>1000011</v>
+        <v>0101111</v>
       </c>
       <c r="G8" s="18" t="str">
         <f t="shared" si="1"/>
-        <v>101001</v>
+        <v>000000</v>
       </c>
       <c r="H8" s="18" t="str">
         <f t="shared" si="1"/>
@@ -7792,11 +7792,11 @@
       </c>
       <c r="B9" s="18">
         <f t="shared" ref="B9:G9" ca="1" si="2">SUMPRODUCT(--MID(B8,LEN(B8)+1-ROW(INDIRECT("1:"&amp;LEN(B8))),1),(2^(ROW(INDIRECT("1:"&amp;LEN(B8)))-1)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C9" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>199</v>
+        <v>5</v>
       </c>
       <c r="D9" s="18">
         <f t="shared" ca="1" si="2"/>
@@ -7804,15 +7804,15 @@
       </c>
       <c r="E9" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F9" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="G9" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
@@ -7830,11 +7830,11 @@
       </c>
       <c r="B10" s="20">
         <f t="shared" ref="B10:O10" ca="1" si="3">B9*B12+B15</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C10" s="20">
         <f t="shared" ca="1" si="3"/>
-        <v>23880</v>
+        <v>600</v>
       </c>
       <c r="D10" s="20">
         <f t="shared" ca="1" si="3"/>
@@ -7842,11 +7842,11 @@
       </c>
       <c r="E10" s="20">
         <f t="shared" ca="1" si="3"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F10" s="20">
         <f t="shared" ca="1" si="3"/>
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="G10" s="20">
         <f t="shared" ca="1" si="3"/>
@@ -8374,11 +8374,11 @@
       </c>
       <c r="B20" s="50">
         <f ca="1">B10</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C20" s="50">
         <f ca="1">C10</f>
-        <v>23880</v>
+        <v>600</v>
       </c>
       <c r="D20" s="50">
         <f ca="1">D10</f>
@@ -8386,11 +8386,11 @@
       </c>
       <c r="E20" s="50">
         <f t="shared" ref="E20:O20" ca="1" si="7">E10</f>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F20" s="50">
         <f t="shared" ca="1" si="7"/>
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="G20" s="50">
         <f t="shared" ca="1" si="7"/>
@@ -8431,40 +8431,40 @@
     </row>
     <row r="21" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="75" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="74" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="74"/>
-      <c r="L22" s="74"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="75"/>
+      <c r="J22" s="75"/>
+      <c r="K22" s="75"/>
+      <c r="L22" s="75"/>
     </row>
     <row r="23" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="74"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="74"/>
-      <c r="L23" s="74"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="75"/>
     </row>
     <row r="24" spans="1:37" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -8484,7 +8484,7 @@
     </row>
     <row r="25" spans="1:37" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="82" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="82"/>
       <c r="C25" s="82"/>
@@ -8500,7 +8500,7 @@
     </row>
     <row r="26" spans="1:37" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -8515,20 +8515,20 @@
       <c r="L26" s="3"/>
     </row>
     <row r="27" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="75" t="s">
+      <c r="A27" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="75"/>
-      <c r="K27" s="75"/>
-      <c r="L27" s="75"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="68"/>
     </row>
     <row r="28" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -8545,18 +8545,18 @@
       <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:37" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="70"/>
-      <c r="B29" s="70"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="70"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="70"/>
-      <c r="J29" s="70"/>
-      <c r="K29" s="70"/>
-      <c r="L29" s="70"/>
+      <c r="A29" s="69"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="69"/>
+      <c r="J29" s="69"/>
+      <c r="K29" s="69"/>
+      <c r="L29" s="69"/>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
@@ -8576,33 +8576,33 @@
       <c r="R30" s="6"/>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A31" s="76" t="s">
+      <c r="A31" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="76"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="76"/>
-      <c r="H31" s="76"/>
-      <c r="I31" s="76"/>
-      <c r="J31" s="76"/>
-      <c r="K31" s="76"/>
-      <c r="L31" s="76"/>
-      <c r="M31" s="76"/>
-      <c r="N31" s="76"/>
-      <c r="O31" s="76"/>
-      <c r="P31" s="76"/>
-      <c r="Q31" s="76"/>
-      <c r="R31" s="76"/>
-      <c r="S31" s="76"/>
-      <c r="T31" s="76"/>
-      <c r="U31" s="76"/>
-      <c r="V31" s="76"/>
-      <c r="W31" s="76"/>
-      <c r="X31" s="76"/>
-      <c r="Y31" s="76"/>
+      <c r="B31" s="70"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="70"/>
+      <c r="J31" s="70"/>
+      <c r="K31" s="70"/>
+      <c r="L31" s="70"/>
+      <c r="M31" s="70"/>
+      <c r="N31" s="70"/>
+      <c r="O31" s="70"/>
+      <c r="P31" s="70"/>
+      <c r="Q31" s="70"/>
+      <c r="R31" s="70"/>
+      <c r="S31" s="70"/>
+      <c r="T31" s="70"/>
+      <c r="U31" s="70"/>
+      <c r="V31" s="70"/>
+      <c r="W31" s="70"/>
+      <c r="X31" s="70"/>
+      <c r="Y31" s="70"/>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -8723,55 +8723,55 @@
       </c>
       <c r="B33" s="55" t="str">
         <f t="shared" ref="B33:AK33" si="8">MID($B4,B32,1)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v>F</v>
+        <v>B</v>
       </c>
       <c r="E33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v>A</v>
+        <v>0</v>
       </c>
       <c r="F33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>B</v>
       </c>
       <c r="H33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v>E</v>
+        <v>C</v>
       </c>
       <c r="I33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v>B</v>
+        <v>0</v>
       </c>
       <c r="K33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="M33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="O33" s="55" t="str">
         <f t="shared" si="8"/>
@@ -8779,43 +8779,43 @@
       </c>
       <c r="P33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="Q33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="R33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="S33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="T33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="U33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="V33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="W33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="X33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="Y33" s="55" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="Z33" s="55" t="str">
         <f t="shared" si="8"/>
@@ -8872,55 +8872,55 @@
       </c>
       <c r="B34" s="54" t="str">
         <f t="shared" ref="B34:AK34" si="9">HEX2BIN(B33,4)</f>
-        <v>0001</v>
+        <v>1000</v>
       </c>
       <c r="C34" s="54" t="str">
         <f t="shared" si="9"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="D34" s="54" t="str">
         <f t="shared" si="9"/>
-        <v>1111</v>
+        <v>1011</v>
       </c>
       <c r="E34" s="54" t="str">
         <f t="shared" si="9"/>
-        <v>1010</v>
+        <v>0000</v>
       </c>
       <c r="F34" s="54" t="str">
         <f t="shared" si="9"/>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="G34" s="54" t="str">
         <f t="shared" si="9"/>
-        <v>0000</v>
+        <v>1011</v>
       </c>
       <c r="H34" s="54" t="str">
         <f t="shared" si="9"/>
-        <v>1110</v>
+        <v>1100</v>
       </c>
       <c r="I34" s="54" t="str">
         <f t="shared" si="9"/>
-        <v>1001</v>
+        <v>0000</v>
       </c>
       <c r="J34" s="54" t="str">
         <f t="shared" si="9"/>
-        <v>1011</v>
+        <v>0000</v>
       </c>
       <c r="K34" s="54" t="str">
         <f t="shared" si="9"/>
-        <v>0011</v>
+        <v>0000</v>
       </c>
       <c r="L34" s="54" t="str">
         <f t="shared" si="9"/>
-        <v>1001</v>
+        <v>0000</v>
       </c>
       <c r="M34" s="54" t="str">
         <f t="shared" si="9"/>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="N34" s="54" t="str">
         <f t="shared" si="9"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="O34" s="54" t="str">
         <f t="shared" si="9"/>
@@ -9033,26 +9033,26 @@
       <c r="P35" s="53"/>
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A36" s="77" t="s">
+      <c r="A36" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="77"/>
-      <c r="C36" s="78" t="s">
+      <c r="B36" s="71"/>
+      <c r="C36" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="D36" s="78"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="79" t="s">
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="G36" s="79"/>
-      <c r="H36" s="78" t="s">
+      <c r="G36" s="73"/>
+      <c r="H36" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="I36" s="78"/>
-      <c r="J36" s="78"/>
-      <c r="K36" s="78"/>
-      <c r="L36" s="78"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="72"/>
+      <c r="K36" s="72"/>
+      <c r="L36" s="72"/>
       <c r="M36" s="53"/>
       <c r="N36" s="53"/>
       <c r="O36" s="53"/>
@@ -9069,12 +9069,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B5:O5"/>
-    <mergeCell ref="A22:L22"/>
     <mergeCell ref="A25:L25"/>
     <mergeCell ref="A27:L27"/>
     <mergeCell ref="A29:L29"/>
@@ -9083,6 +9077,12 @@
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="H36:L36"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B5:O5"/>
+    <mergeCell ref="A22:L22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C36" r:id="rId1" xr:uid="{91A7F21F-D12F-4016-99B6-B5719B516BED}"/>
@@ -9101,7 +9101,7 @@
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:O5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9121,50 +9121,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
     </row>
     <row r="2" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
@@ -9179,20 +9179,20 @@
       <c r="Y2" s="7"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="56"/>
@@ -9212,7 +9212,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C4" s="57"/>
       <c r="D4" s="57"/>
@@ -9230,23 +9230,23 @@
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="72" t="str">
+      <c r="B5" s="79" t="str">
         <f>CONCATENATE(B34,C34,D34,E34,F34,G34,H34,I34,J34,K34,L34,M34,N34,O34,P34,Q34,R34,S34,T34,U34,V34,W34,X34,Y34,Z34,AA34,AB34,AC34,AD34,AE34,AF34,AG34,AH34,AI34,AJ34,AK34)</f>
         <v>000010000100110100000011010011011001100000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -9329,7 +9329,7 @@
         <v>20</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H7" s="17"/>
       <c r="J7" s="17"/>
@@ -9512,10 +9512,10 @@
         <v>28</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" s="24" t="s">
         <v>31</v>
@@ -10047,40 +10047,40 @@
     </row>
     <row r="21" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="75" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="74" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="74"/>
-      <c r="L22" s="74"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="75"/>
+      <c r="J22" s="75"/>
+      <c r="K22" s="75"/>
+      <c r="L22" s="75"/>
     </row>
     <row r="23" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="74"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="74"/>
-      <c r="L23" s="74"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="75"/>
     </row>
     <row r="24" spans="1:37" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -10100,7 +10100,7 @@
     </row>
     <row r="25" spans="1:37" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="82" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="82"/>
       <c r="C25" s="82"/>
@@ -10116,7 +10116,7 @@
     </row>
     <row r="26" spans="1:37" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -10131,20 +10131,20 @@
       <c r="L26" s="3"/>
     </row>
     <row r="27" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="75" t="s">
+      <c r="A27" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="75"/>
-      <c r="J27" s="75"/>
-      <c r="K27" s="75"/>
-      <c r="L27" s="75"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="68"/>
     </row>
     <row r="28" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -10161,18 +10161,18 @@
       <c r="L28" s="3"/>
     </row>
     <row r="29" spans="1:37" s="60" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="70"/>
-      <c r="B29" s="70"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="70"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="70"/>
-      <c r="J29" s="70"/>
-      <c r="K29" s="70"/>
-      <c r="L29" s="70"/>
+      <c r="A29" s="69"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="69"/>
+      <c r="J29" s="69"/>
+      <c r="K29" s="69"/>
+      <c r="L29" s="69"/>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
@@ -10192,33 +10192,33 @@
       <c r="R30" s="6"/>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A31" s="76" t="s">
+      <c r="A31" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="76"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="76"/>
-      <c r="H31" s="76"/>
-      <c r="I31" s="76"/>
-      <c r="J31" s="76"/>
-      <c r="K31" s="76"/>
-      <c r="L31" s="76"/>
-      <c r="M31" s="76"/>
-      <c r="N31" s="76"/>
-      <c r="O31" s="76"/>
-      <c r="P31" s="76"/>
-      <c r="Q31" s="76"/>
-      <c r="R31" s="76"/>
-      <c r="S31" s="76"/>
-      <c r="T31" s="76"/>
-      <c r="U31" s="76"/>
-      <c r="V31" s="76"/>
-      <c r="W31" s="76"/>
-      <c r="X31" s="76"/>
-      <c r="Y31" s="76"/>
+      <c r="B31" s="70"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="70"/>
+      <c r="J31" s="70"/>
+      <c r="K31" s="70"/>
+      <c r="L31" s="70"/>
+      <c r="M31" s="70"/>
+      <c r="N31" s="70"/>
+      <c r="O31" s="70"/>
+      <c r="P31" s="70"/>
+      <c r="Q31" s="70"/>
+      <c r="R31" s="70"/>
+      <c r="S31" s="70"/>
+      <c r="T31" s="70"/>
+      <c r="U31" s="70"/>
+      <c r="V31" s="70"/>
+      <c r="W31" s="70"/>
+      <c r="X31" s="70"/>
+      <c r="Y31" s="70"/>
     </row>
     <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
@@ -10649,26 +10649,26 @@
       <c r="P35" s="53"/>
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A36" s="77" t="s">
+      <c r="A36" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="77"/>
-      <c r="C36" s="78" t="s">
+      <c r="B36" s="71"/>
+      <c r="C36" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="D36" s="78"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="79" t="s">
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="G36" s="79"/>
-      <c r="H36" s="78" t="s">
+      <c r="G36" s="73"/>
+      <c r="H36" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="I36" s="78"/>
-      <c r="J36" s="78"/>
-      <c r="K36" s="78"/>
-      <c r="L36" s="78"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="72"/>
+      <c r="K36" s="72"/>
+      <c r="L36" s="72"/>
       <c r="M36" s="53"/>
       <c r="N36" s="53"/>
       <c r="O36" s="53"/>
@@ -10685,6 +10685,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B5:O5"/>
+    <mergeCell ref="A22:L22"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="C36:E36"/>
     <mergeCell ref="F36:G36"/>
@@ -10694,11 +10699,6 @@
     <mergeCell ref="A27:L27"/>
     <mergeCell ref="A29:L29"/>
     <mergeCell ref="A31:Y31"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B5:O5"/>
-    <mergeCell ref="A22:L22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C36" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -10740,50 +10740,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
+      <c r="A1" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
     </row>
     <row r="2" spans="1:25" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
@@ -10798,20 +10798,20 @@
       <c r="Y2" s="7"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
@@ -10830,41 +10830,41 @@
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="72" t="str">
+      <c r="B5" s="79" t="str">
         <f>CONCATENATE(B40,C40,D40,E40,F40,G40,H40,I40,J40,K40,L40,M40,N40,O40,P40,Q40,R40,S40,T40,U40,V40,W40,X40,Y40,Z40,AA40,AB40,AC40,AD40,AE40,AF40,AG40,AH40,AI40,AJ40,AK40)</f>
         <v>001010100110001000011001101100101100100001001111111111001001010111101001011000110010001100011000101011111001111100000000000000000000000000000000</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -11716,20 +11716,20 @@
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" s="73" t="s">
+      <c r="A21" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="73"/>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="73"/>
-      <c r="L21" s="73"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="74"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
+      <c r="K21" s="74"/>
+      <c r="L21" s="74"/>
       <c r="M21" s="51"/>
       <c r="N21" s="51"/>
       <c r="O21" s="51"/>
@@ -11774,20 +11774,20 @@
       <c r="Y22" s="51"/>
     </row>
     <row r="23" spans="1:25" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
-      <c r="I23" s="74"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="74"/>
-      <c r="L23" s="74"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="75"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="75"/>
       <c r="M23" s="83" t="s">
         <v>66</v>
       </c>
@@ -11805,20 +11805,20 @@
       <c r="Y23" s="83"/>
     </row>
     <row r="24" spans="1:25" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="74" t="s">
+      <c r="A24" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="74"/>
-      <c r="K24" s="74"/>
-      <c r="L24" s="74"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
+      <c r="J24" s="75"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="75"/>
       <c r="M24" s="83"/>
       <c r="N24" s="83"/>
       <c r="O24" s="83"/>
@@ -11834,20 +11834,20 @@
       <c r="Y24" s="83"/>
     </row>
     <row r="25" spans="1:25" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="74" t="s">
+      <c r="A25" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="74"/>
-      <c r="K25" s="74"/>
-      <c r="L25" s="74"/>
+      <c r="B25" s="75"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="75"/>
+      <c r="K25" s="75"/>
+      <c r="L25" s="75"/>
       <c r="M25" s="83"/>
       <c r="N25" s="83"/>
       <c r="O25" s="83"/>
@@ -12040,50 +12040,50 @@
       <c r="L32" s="3"/>
     </row>
     <row r="33" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="70" t="s">
+      <c r="A33" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="70"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="70"/>
-      <c r="H33" s="70"/>
-      <c r="I33" s="70"/>
-      <c r="J33" s="70"/>
-      <c r="K33" s="70"/>
-      <c r="L33" s="70"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="69"/>
+      <c r="J33" s="69"/>
+      <c r="K33" s="69"/>
+      <c r="L33" s="69"/>
     </row>
     <row r="34" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="75" t="s">
+      <c r="A34" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="75"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="75"/>
-      <c r="J34" s="75"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="75"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="68"/>
+      <c r="J34" s="68"/>
+      <c r="K34" s="68"/>
+      <c r="L34" s="68"/>
     </row>
     <row r="35" spans="1:37" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="70"/>
-      <c r="B35" s="70"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="70"/>
-      <c r="F35" s="70"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="70"/>
-      <c r="K35" s="70"/>
-      <c r="L35" s="70"/>
+      <c r="A35" s="69"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="69"/>
     </row>
     <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
@@ -12103,33 +12103,33 @@
       <c r="R36" s="6"/>
     </row>
     <row r="37" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A37" s="76" t="s">
+      <c r="A37" s="70" t="s">
         <v>58</v>
       </c>
-      <c r="B37" s="76"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="76"/>
-      <c r="H37" s="76"/>
-      <c r="I37" s="76"/>
-      <c r="J37" s="76"/>
-      <c r="K37" s="76"/>
-      <c r="L37" s="76"/>
-      <c r="M37" s="76"/>
-      <c r="N37" s="76"/>
-      <c r="O37" s="76"/>
-      <c r="P37" s="76"/>
-      <c r="Q37" s="76"/>
-      <c r="R37" s="76"/>
-      <c r="S37" s="76"/>
-      <c r="T37" s="76"/>
-      <c r="U37" s="76"/>
-      <c r="V37" s="76"/>
-      <c r="W37" s="76"/>
-      <c r="X37" s="76"/>
-      <c r="Y37" s="76"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="70"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="70"/>
+      <c r="L37" s="70"/>
+      <c r="M37" s="70"/>
+      <c r="N37" s="70"/>
+      <c r="O37" s="70"/>
+      <c r="P37" s="70"/>
+      <c r="Q37" s="70"/>
+      <c r="R37" s="70"/>
+      <c r="S37" s="70"/>
+      <c r="T37" s="70"/>
+      <c r="U37" s="70"/>
+      <c r="V37" s="70"/>
+      <c r="W37" s="70"/>
+      <c r="X37" s="70"/>
+      <c r="Y37" s="70"/>
     </row>
     <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -12560,26 +12560,26 @@
       <c r="P41" s="53"/>
     </row>
     <row r="42" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A42" s="77" t="s">
+      <c r="A42" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="B42" s="77"/>
-      <c r="C42" s="78" t="s">
+      <c r="B42" s="71"/>
+      <c r="C42" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="78"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="79" t="s">
+      <c r="D42" s="72"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="G42" s="79"/>
-      <c r="H42" s="78" t="s">
+      <c r="G42" s="73"/>
+      <c r="H42" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="I42" s="78"/>
-      <c r="J42" s="78"/>
-      <c r="K42" s="78"/>
-      <c r="L42" s="78"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="72"/>
+      <c r="L42" s="72"/>
       <c r="M42" s="53"/>
       <c r="N42" s="53"/>
       <c r="O42" s="53"/>
@@ -12596,6 +12596,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:Y1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="B5:O5"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="M23:Y30"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A25:L25"/>
     <mergeCell ref="A33:L33"/>
     <mergeCell ref="A34:L34"/>
     <mergeCell ref="A35:L35"/>
@@ -12604,16 +12614,6 @@
     <mergeCell ref="C42:E42"/>
     <mergeCell ref="F42:G42"/>
     <mergeCell ref="H42:L42"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="M23:Y30"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="A1:Y1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="B5:O5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C42" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -12634,33 +12634,33 @@
   <sheetData>
     <row r="1" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>